<commit_message>
chore: update base code
</commit_message>
<xml_diff>
--- a/sites.xlsx
+++ b/sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bassfredes\Proyectos\2025\Forus\AutoReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A027B9B5-373F-4474-9D43-70BF08A893F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3C82E3-B1AD-4D4A-A0A7-B4DC50B494B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="2820" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31830" yWindow="2145" windowWidth="22215" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>url</t>
   </si>
   <si>
-    <t>https://www.columbiachile.cl/</t>
-  </si>
-  <si>
-    <t>https://www.columbiachile.cl/Hombre</t>
-  </si>
-  <si>
-    <t>https://www.columbiachile.cl/chaqueta-unisex-ycsc-x-disney-mickey-columbia-2125161-xp9/p</t>
-  </si>
-  <si>
-    <t>https://www.columbiachile.cl/checkout/?orderFormId=99283ff6f1e945a1bd1ff9eab700ed6a#/cart</t>
+    <t>https://www.zapatos.cl/</t>
+  </si>
+  <si>
+    <t>https://www.zapatos.cl/?__disablePixels</t>
+  </si>
+  <si>
+    <t>https://www.zapatos.cl/mujer?map=genero</t>
+  </si>
+  <si>
+    <t>https://www.zapatos.cl/mujer?map=genero?__disablePixels</t>
+  </si>
+  <si>
+    <t>https://www.zapatos.cl/polera-m-c-mujer-v-neck-bsoul-bs210021428-7un/p</t>
+  </si>
+  <si>
+    <t>https://www.zapatos.cl/polera-m-c-mujer-v-neck-bsoul-bs210021428-7un/p?__disablePixels</t>
+  </si>
+  <si>
+    <t>https://www.zapatos.cl/checkout/?orderFormId=f90f4001500640a9a603a60e61c61d60#/cart</t>
   </si>
 </sst>
 </file>
@@ -81,7 +90,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -387,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,21 +418,37 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>